<commit_message>
updates to code and new pdf
</commit_message>
<xml_diff>
--- a/data/derived/arc-tme-ornl/co2Flux_ornl_sum_2020-04-13.xlsx
+++ b/data/derived/arc-tme-ornl/co2Flux_ornl_sum_2020-04-13.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" hidePivotFieldList="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1700" yWindow="40" windowWidth="25040" windowHeight="16860" tabRatio="500" activeTab="5"/>
+    <workbookView xWindow="6440" yWindow="0" windowWidth="21620" windowHeight="16860" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <pivotCaches>
-    <pivotCache cacheId="15" r:id="rId8"/>
+    <pivotCache cacheId="1" r:id="rId8"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -4158,7 +4158,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="15" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
   <location ref="A1:O16" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
   <pivotFields count="18">
     <pivotField showAll="0"/>
@@ -15497,7 +15497,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE56"/>
   <sheetViews>
-    <sheetView topLeftCell="R1" workbookViewId="0">
+    <sheetView topLeftCell="O1" workbookViewId="0">
       <selection activeCell="AB4" sqref="A4:AB4"/>
     </sheetView>
   </sheetViews>
@@ -18276,8 +18276,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G13"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="T2" sqref="T2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -18417,8 +18417,8 @@
         <v>-26.444909450000001</v>
       </c>
       <c r="S2">
-        <f>VLOOKUP($C2,d14C!$C$4:$AB$27,26,FALSE)</f>
-        <v>205.96492402693255</v>
+        <f>VLOOKUP($C2,d14C!$Y$4:$AB$27,4,FALSE)</f>
+        <v>380.88596619884549</v>
       </c>
     </row>
     <row r="3" spans="1:19">
@@ -18488,8 +18488,8 @@
         <v>-27.458819399999999</v>
       </c>
       <c r="S3">
-        <f>VLOOKUP($C3,d14C!$C$4:$AB$27,26,FALSE)</f>
-        <v>196.65185208148773</v>
+        <f>VLOOKUP($C3,d14C!$Y$4:$AB$27,4,FALSE)</f>
+        <v>315.64760764651891</v>
       </c>
     </row>
     <row r="4" spans="1:19">
@@ -18559,8 +18559,8 @@
         <v>-26.296340749999999</v>
       </c>
       <c r="S4">
-        <f>VLOOKUP($C4,d14C!$C$4:$AB$27,26,FALSE)</f>
-        <v>185.735362801267</v>
+        <f>VLOOKUP($C4,d14C!$Y$4:$AB$27,4,FALSE)</f>
+        <v>412.71385456572563</v>
       </c>
     </row>
     <row r="5" spans="1:19">
@@ -18630,8 +18630,8 @@
         <v>-27.667189775000004</v>
       </c>
       <c r="S5">
-        <f>VLOOKUP($C5,d14C!$C$4:$AB$27,26,FALSE)</f>
-        <v>153.92421436218328</v>
+        <f>VLOOKUP($C5,d14C!$Y$4:$AB$27,4,FALSE)</f>
+        <v>319.79482839457131</v>
       </c>
     </row>
     <row r="6" spans="1:19">
@@ -18701,8 +18701,8 @@
         <v>-26.629163250000001</v>
       </c>
       <c r="S6">
-        <f>VLOOKUP($C6,d14C!$C$4:$AB$27,26,FALSE)</f>
-        <v>174.96701076591293</v>
+        <f>VLOOKUP($C6,d14C!$Y$4:$AB$27,4,FALSE)</f>
+        <v>347.73401064483522</v>
       </c>
     </row>
     <row r="7" spans="1:19">
@@ -18772,8 +18772,8 @@
         <v>-25.338596350000003</v>
       </c>
       <c r="S7">
-        <f>VLOOKUP($C7,d14C!$C$4:$AB$27,26,FALSE)</f>
-        <v>167.48153302296399</v>
+        <f>VLOOKUP($C7,d14C!$Y$4:$AB$27,4,FALSE)</f>
+        <v>335.4465593989899</v>
       </c>
     </row>
     <row r="8" spans="1:19">
@@ -18843,8 +18843,8 @@
         <v>-27.224269750000001</v>
       </c>
       <c r="S8">
-        <f>VLOOKUP($C8,d14C!$C$4:$AB$27,26,FALSE)</f>
-        <v>380.88596619884549</v>
+        <f>VLOOKUP($C8,d14C!$Y$4:$AB$27,4,FALSE)</f>
+        <v>205.96492402693255</v>
       </c>
     </row>
     <row r="9" spans="1:19">
@@ -18914,8 +18914,8 @@
         <v>-27.717386600000001</v>
       </c>
       <c r="S9">
-        <f>VLOOKUP($C9,d14C!$C$4:$AB$27,26,FALSE)</f>
-        <v>254.86760860379621</v>
+        <f>VLOOKUP($C9,d14C!$Y$4:$AB$27,4,FALSE)</f>
+        <v>185.735362801267</v>
       </c>
     </row>
     <row r="10" spans="1:19">
@@ -18985,8 +18985,8 @@
         <v>-26.823392500000001</v>
       </c>
       <c r="S10">
-        <f>VLOOKUP($C10,d14C!$C$4:$AB$27,26,FALSE)</f>
-        <v>315.64760764651891</v>
+        <f>VLOOKUP($C10,d14C!$Y$4:$AB$27,4,FALSE)</f>
+        <v>174.96701076591293</v>
       </c>
     </row>
     <row r="11" spans="1:19">
@@ -19056,8 +19056,8 @@
         <v>-27.942159575000002</v>
       </c>
       <c r="S11">
-        <f>VLOOKUP($C11,d14C!$C$4:$AB$27,26,FALSE)</f>
-        <v>233.94798760744573</v>
+        <f>VLOOKUP($C11,d14C!$Y$4:$AB$27,4,FALSE)</f>
+        <v>174.6750956370835</v>
       </c>
     </row>
     <row r="12" spans="1:19">
@@ -19127,8 +19127,8 @@
         <v>-27.600948900000006</v>
       </c>
       <c r="S12">
-        <f>VLOOKUP($C12,d14C!$C$4:$AB$27,26,FALSE)</f>
-        <v>412.71385456572563</v>
+        <f>VLOOKUP($C12,d14C!$Y$4:$AB$27,4,FALSE)</f>
+        <v>214.01132546765123</v>
       </c>
     </row>
     <row r="13" spans="1:19">
@@ -19198,8 +19198,8 @@
         <v>-28.776365125000002</v>
       </c>
       <c r="S13">
-        <f>VLOOKUP($C13,d14C!$C$4:$AB$27,26,FALSE)</f>
-        <v>385.06930973413444</v>
+        <f>VLOOKUP($C13,d14C!$Y$4:$AB$27,4,FALSE)</f>
+        <v>204.63133849046255</v>
       </c>
     </row>
   </sheetData>

</xml_diff>